<commit_message>
✨ Add image gallery + sizes parsing and display
Parser improvements:
- Added sizes parsing from TradeInn (multiple methods)
- Parse sizes for shoes, clothes, accessories
- Extract all product images for gallery

Mini App improvements:
- Image gallery with navigation arrows (swipe between photos)
- Display available sizes in modal window
- Load sizes and all images from Excel
- Beautiful size badges with hover effects
- Gallery counter showing current photo number

UX improvements:
- Smooth transitions between photos
- Size badges in grid layout
- Navigation arrows appear only when multiple photos
- Auto-hide gallery controls for single image products
</commit_message>
<xml_diff>
--- a/products_links.xlsx
+++ b/products_links.xlsx
@@ -1,41 +1,138 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hovo\OneDrive\Desktop\minin app\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D84F961-83AE-4CFB-8366-1F4394CB8781}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="🛍 Товары" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="🛍 Товары" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'🛍 Товары'!$A$1:$K$1</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+  <si>
+    <t>URL товара</t>
+  </si>
+  <si>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>Цена (€)</t>
+  </si>
+  <si>
+    <t>Описание</t>
+  </si>
+  <si>
+    <t>Группа</t>
+  </si>
+  <si>
+    <t>Подгруппа</t>
+  </si>
+  <si>
+    <t>URL фото</t>
+  </si>
+  <si>
+    <t>Локальное фото</t>
+  </si>
+  <si>
+    <t>Размеры</t>
+  </si>
+  <si>
+    <t>Последнее обновление</t>
+  </si>
+  <si>
+    <t>Статус</t>
+  </si>
+  <si>
+    <t>https://www.tradeinn.com/smashinn/en/bullpadel-vertex-04-2025-padel-racket/141382757/p?utm_source=google_buscador&amp;utm_medium=google_buscador&amp;attributionToken=mwHwmgoMCJ_ZuMwGEOL9gdQDEAEaJDY5Yzg2MGM0LTAwMDAtMjMzZS1iMWYyLTA0MDA2ZTZmYjg1MCoVMTUxODIwODUzNi4xNzcwOTI1MjE1MjCOvp0V6avYN6jlqi2b1rctjpHJMPbd8Te3t4wtjsCPN9SynRXC8J4VmNa3LZD3sjA6DmRlZmF1bHRfc2VhcmNoSAFYAWgBcAF6Andh</t>
+  </si>
+  <si>
+    <t>Bullpadel ракетка для паделя Vertex 04 2025</t>
+  </si>
+  <si>
+    <t>Получите Bullpadel Vertex 04 2025 в цвете  Серебристый за 176.99 €. Отлично для теннис и весло, быст</t>
+  </si>
+  <si>
+    <t>https://www.tradeinn.com/f/14138/141382757/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_2/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_3/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_4/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_5/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_6/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_7/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_8/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_9/bullpadel-ракетка-для-паделя-vertex-04-2025.webp</t>
+  </si>
+  <si>
+    <t>images\product_1_399.webp, images\product_1_6100.webp, images\product_1_4293.webp, images\product_1_5561.webp, images\product_1_3529.webp, images\product_1_8657.webp, images\product_1_8450.webp, images\product_1_2614.webp, images\product_1_1736.webp</t>
+  </si>
+  <si>
+    <t>2026-02-13 21:33</t>
+  </si>
+  <si>
+    <t>✅ Обновлено</t>
+  </si>
+  <si>
+    <t>https://www.tradeinn.com/volleyball/ru/asics-%D0%9E%D0%B1%D1%83%D0%B2%D1%8C-%D0%B4%D0%BB%D1%8F-%D0%B7%D0%B0%D0%BA%D1%80%D1%8B%D1%82%D1%8B%D1%85-%D0%BA%D0%BE%D1%80%D1%82%D0%BE%D0%B2-netburner-ballistic-ff-3/141608258/p</t>
+  </si>
+  <si>
+    <t>Asics Обувь для закрытых кортов Netburner Ballistic FF 3</t>
+  </si>
+  <si>
+    <t>Получите Asics Netburner Ballistic FF 3 в цвете  Белая за 78 €. Отлично для Волейбол, быстрая достав</t>
+  </si>
+  <si>
+    <t>https://www.tradeinn.com/f/14160/141608258/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_2/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_3/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_4/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_5/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_6/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_7/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp</t>
+  </si>
+  <si>
+    <t>images\product_2_5309.webp, images\product_2_9387.webp, images\product_2_7678.webp, images\product_2_8904.webp, images\product_2_799.webp, images\product_2_7971.webp, images\product_2_1069.webp</t>
+  </si>
+  <si>
+    <t>2026-02-13 21:34</t>
+  </si>
+  <si>
+    <t>Обувь</t>
+  </si>
+  <si>
+    <t>для волейбола</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <b val="1"/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="14"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -71,87 +168,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -439,170 +480,125 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="55" customWidth="1" min="1" max="1"/>
-    <col width="35" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="45" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="6"/>
-    <col width="45" customWidth="1" min="7" max="7"/>
-    <col width="25" customWidth="1" min="8" max="9"/>
-    <col width="22" customWidth="1" min="10" max="10"/>
-    <col width="18" customWidth="1" min="11" max="11"/>
+    <col min="1" max="1" width="55" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="45" customWidth="1"/>
+    <col min="5" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="45" customWidth="1"/>
+    <col min="8" max="9" width="25" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>URL товара</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Название</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Цена (€)</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Описание</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Группа</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Подгруппа</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>URL фото</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Локальное фото</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Размеры</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Последнее обновление</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Статус</t>
-        </is>
+    <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>https://www.tradeinn.com/smashinn/en/bullpadel-vertex-04-2025-padel-racket/141382757/p?utm_source=google_buscador&amp;utm_medium=google_buscador&amp;attributionToken=mwHwmgoMCJ_ZuMwGEOL9gdQDEAEaJDY5Yzg2MGM0LTAwMDAtMjMzZS1iMWYyLTA0MDA2ZTZmYjg1MCoVMTUxODIwODUzNi4xNzcwOTI1MjE1MjCOvp0V6avYN6jlqi2b1rctjpHJMPbd8Te3t4wtjsCPN9SynRXC8J4VmNa3LZD3sjA6DmRlZmF1bHRfc2VhcmNoSAFYAWgBcAF6Andh</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Bullpadel ракетка для паделя Vertex 04 2025</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
         <v>176.99</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Получите Bullpadel Vertex 04 2025 в цвете  Серебристый за 176.99 €. Отлично для теннис и весло, быст</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>https://www.tradeinn.com/f/14138/141382757/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_2/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_3/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_4/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_5/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_6/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_7/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_8/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_9/bullpadel-ракетка-для-паделя-vertex-04-2025.webp</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>images\product_1_399.webp, images\product_1_6100.webp, images\product_1_4293.webp, images\product_1_5561.webp, images\product_1_3529.webp, images\product_1_8657.webp, images\product_1_8450.webp, images\product_1_2614.webp, images\product_1_1736.webp</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>2026-02-13 21:33</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>✅ Обновлено</t>
-        </is>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>https://www.tradeinn.com/volleyball/ru/asics-%D0%9E%D0%B1%D1%83%D0%B2%D1%8C-%D0%B4%D0%BB%D1%8F-%D0%B7%D0%B0%D0%BA%D1%80%D1%8B%D1%82%D1%8B%D1%85-%D0%BA%D0%BE%D1%80%D1%82%D0%BE%D0%B2-netburner-ballistic-ff-3/141608258/p</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Asics Обувь для закрытых кортов Netburner Ballistic FF 3</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
         <v>78</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Получите Asics Netburner Ballistic FF 3 в цвете  Белая за 78 €. Отлично для Волейбол, быстрая достав</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>https://www.tradeinn.com/f/14160/141608258/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_2/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_3/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_4/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_5/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_6/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_7/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>images\product_2_5309.webp, images\product_2_9387.webp, images\product_2_7678.webp, images\product_2_8904.webp, images\product_2_799.webp, images\product_2_7971.webp, images\product_2_1069.webp</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>2026-02-13 21:34</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>✅ Обновлено</t>
-        </is>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K1"/>
+  <autoFilter ref="A1:K1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{3BEB3070-C6A5-416C-B57F-94CBDB094083}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
🎯 Optimize: Download only first photo per product
Major optimization for large catalogs (1000+ products):

Parser changes:
- Download ONLY first photo instead of all photos
- Saves bandwidth and disk space
- Faster parsing (5-10x for re-parsing)
- For 1000 products: 1000 files instead of 10000+

Mini App changes:
- Removed image gallery (arrows, counter)
- Simplified JavaScript (no changeModalImage function)
- Show only single product image in modal
- Cleaner, simpler UI

Benefits:
- Much smaller images folder
- Faster deployment to Amvera
- Less traffic on updates
- One photo is enough for catalog view
</commit_message>
<xml_diff>
--- a/products_links.xlsx
+++ b/products_links.xlsx
@@ -1,138 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hovo\OneDrive\Desktop\minin app\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D84F961-83AE-4CFB-8366-1F4394CB8781}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="🛍 Товары" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="🛍 Товары" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'🛍 Товары'!$A$1:$K$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
-  <si>
-    <t>URL товара</t>
-  </si>
-  <si>
-    <t>Название</t>
-  </si>
-  <si>
-    <t>Цена (€)</t>
-  </si>
-  <si>
-    <t>Описание</t>
-  </si>
-  <si>
-    <t>Группа</t>
-  </si>
-  <si>
-    <t>Подгруппа</t>
-  </si>
-  <si>
-    <t>URL фото</t>
-  </si>
-  <si>
-    <t>Локальное фото</t>
-  </si>
-  <si>
-    <t>Размеры</t>
-  </si>
-  <si>
-    <t>Последнее обновление</t>
-  </si>
-  <si>
-    <t>Статус</t>
-  </si>
-  <si>
-    <t>https://www.tradeinn.com/smashinn/en/bullpadel-vertex-04-2025-padel-racket/141382757/p?utm_source=google_buscador&amp;utm_medium=google_buscador&amp;attributionToken=mwHwmgoMCJ_ZuMwGEOL9gdQDEAEaJDY5Yzg2MGM0LTAwMDAtMjMzZS1iMWYyLTA0MDA2ZTZmYjg1MCoVMTUxODIwODUzNi4xNzcwOTI1MjE1MjCOvp0V6avYN6jlqi2b1rctjpHJMPbd8Te3t4wtjsCPN9SynRXC8J4VmNa3LZD3sjA6DmRlZmF1bHRfc2VhcmNoSAFYAWgBcAF6Andh</t>
-  </si>
-  <si>
-    <t>Bullpadel ракетка для паделя Vertex 04 2025</t>
-  </si>
-  <si>
-    <t>Получите Bullpadel Vertex 04 2025 в цвете  Серебристый за 176.99 €. Отлично для теннис и весло, быст</t>
-  </si>
-  <si>
-    <t>https://www.tradeinn.com/f/14138/141382757/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_2/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_3/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_4/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_5/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_6/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_7/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_8/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_9/bullpadel-ракетка-для-паделя-vertex-04-2025.webp</t>
-  </si>
-  <si>
-    <t>images\product_1_399.webp, images\product_1_6100.webp, images\product_1_4293.webp, images\product_1_5561.webp, images\product_1_3529.webp, images\product_1_8657.webp, images\product_1_8450.webp, images\product_1_2614.webp, images\product_1_1736.webp</t>
-  </si>
-  <si>
-    <t>2026-02-13 21:33</t>
-  </si>
-  <si>
-    <t>✅ Обновлено</t>
-  </si>
-  <si>
-    <t>https://www.tradeinn.com/volleyball/ru/asics-%D0%9E%D0%B1%D1%83%D0%B2%D1%8C-%D0%B4%D0%BB%D1%8F-%D0%B7%D0%B0%D0%BA%D1%80%D1%8B%D1%82%D1%8B%D1%85-%D0%BA%D0%BE%D1%80%D1%82%D0%BE%D0%B2-netburner-ballistic-ff-3/141608258/p</t>
-  </si>
-  <si>
-    <t>Asics Обувь для закрытых кортов Netburner Ballistic FF 3</t>
-  </si>
-  <si>
-    <t>Получите Asics Netburner Ballistic FF 3 в цвете  Белая за 78 €. Отлично для Волейбол, быстрая достав</t>
-  </si>
-  <si>
-    <t>https://www.tradeinn.com/f/14160/141608258/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_2/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_3/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_4/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_5/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_6/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_7/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp</t>
-  </si>
-  <si>
-    <t>images\product_2_5309.webp, images\product_2_9387.webp, images\product_2_7678.webp, images\product_2_8904.webp, images\product_2_799.webp, images\product_2_7971.webp, images\product_2_1069.webp</t>
-  </si>
-  <si>
-    <t>2026-02-13 21:34</t>
-  </si>
-  <si>
-    <t>Обувь</t>
-  </si>
-  <si>
-    <t>для волейбола</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
       <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -168,31 +71,87 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -480,125 +439,176 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55" customWidth="1"/>
-    <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="45" customWidth="1"/>
-    <col min="5" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="45" customWidth="1"/>
-    <col min="8" max="9" width="25" customWidth="1"/>
-    <col min="10" max="10" width="22" customWidth="1"/>
-    <col min="11" max="11" width="18" customWidth="1"/>
+    <col width="55" customWidth="1" min="1" max="1"/>
+    <col width="35" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="45" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="6"/>
+    <col width="45" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="8" max="9"/>
+    <col width="22" customWidth="1" min="10" max="10"/>
+    <col width="18" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
+    <row r="1" ht="30" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>URL товара</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Название</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Цена (€)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Описание</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Группа</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Подгруппа</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>URL фото</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Локальное фото</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Размеры</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Последнее обновление</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Статус</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>https://www.tradeinn.com/smashinn/en/bullpadel-vertex-04-2025-padel-racket/141382757/p?utm_source=google_buscador&amp;utm_medium=google_buscador&amp;attributionToken=mwHwmgoMCJ_ZuMwGEOL9gdQDEAEaJDY5Yzg2MGM0LTAwMDAtMjMzZS1iMWYyLTA0MDA2ZTZmYjg1MCoVMTUxODIwODUzNi4xNzcwOTI1MjE1MjCOvp0V6avYN6jlqi2b1rctjpHJMPbd8Te3t4wtjsCPN9SynRXC8J4VmNa3LZD3sjA6DmRlZmF1bHRfc2VhcmNoSAFYAWgBcAF6Andh</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Bullpadel ракетка для паделя Vertex 04 2025</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>176.99</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Получите Bullpadel Vertex 04 2025 в цвете  Серебристый за 176.99 €. Отлично для теннис и весло, быст</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://www.tradeinn.com/f/14138/141382757/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_2/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_3/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_4/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_5/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_6/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_7/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_8/bullpadel-ракетка-для-паделя-vertex-04-2025.webp, https://www.tradeinn.com/f/14138/141382757_9/bullpadel-ракетка-для-паделя-vertex-04-2025.webp</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>images\product_1_7481.webp, images\product_1_7369.webp, images\product_1_6214.webp, images\product_1_5127.webp, images\product_1_8353.webp, images\product_1_9033.webp, images\product_1_995.webp, images\product_1_5640.webp, images\product_1_5977.webp</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2026-02-13 23:32</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>✅ Обновлено</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>https://www.tradeinn.com/volleyball/ru/asics-%D0%9E%D0%B1%D1%83%D0%B2%D1%8C-%D0%B4%D0%BB%D1%8F-%D0%B7%D0%B0%D0%BA%D1%80%D1%8B%D1%82%D1%8B%D1%85-%D0%BA%D0%BE%D1%80%D1%82%D0%BE%D0%B2-netburner-ballistic-ff-3/141608258/p</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Asics Обувь для закрытых кортов Netburner Ballistic FF 3</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>78</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Получите Asics Netburner Ballistic FF 3 в цвете  Белая за 78 €. Отлично для Волейбол, быстрая достав</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>https://www.tradeinn.com/f/14160/141608258/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_2/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_3/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_4/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_5/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_6/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp, https://www.tradeinn.com/f/14160/141608258_7/asics-Обувь-для-закрытых-кортов-netburner-ballistic-ff-3.webp</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>images\product_2_973.webp, images\product_2_1052.webp, images\product_2_2549.webp, images\product_2_3291.webp, images\product_2_7789.webp, images\product_2_7181.webp, images\product_2_4192.webp</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>40 1/2, 42, 42 1/2, 43 1/2, 44, 44 1/2, 45, 46</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2026-02-13 23:32</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>✅ Обновлено</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{3BEB3070-C6A5-416C-B57F-94CBDB094083}"/>
-  </hyperlinks>
+  <autoFilter ref="A1:K1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>